<commit_message>
Added subscriptionNo18 scenarios and stepdef
</commit_message>
<xml_diff>
--- a/src/test/resources/HerBalance_TestData.xlsx
+++ b/src/test/resources/HerBalance_TestData.xlsx
@@ -3,25 +3,44 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Onboarding" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Menstrual Phase Logs" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="SignUp" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Onboarding" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Menstrual Phase Logs" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="LP2CBb1Am8XbDvG1Rpml9Fd3xJX3SSEUlTv6RYbBKqQ="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="ursbU7wlYnP9eQyEL312XInmeImyLslS6QLJXZUpuDw="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Key</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>team2surfers@gmail.com</t>
+  </si>
+  <si>
+    <t>Team@123</t>
+  </si>
+  <si>
     <t>Last Period Date</t>
   </si>
   <si>
@@ -31,7 +50,7 @@
     <t>Menstrual Data</t>
   </si>
   <si>
-    <t>01/14/2026</t>
+    <t>01/28/2026</t>
   </si>
   <si>
     <t>Details</t>
@@ -65,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -77,6 +96,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Sans-serif"/>
     </font>
     <font>
       <color theme="1"/>
@@ -127,32 +151,35 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -168,6 +195,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -375,9 +406,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.38"/>
-    <col customWidth="1" min="2" max="2" width="14.13"/>
-    <col customWidth="1" min="3" max="3" width="13.5"/>
+    <col customWidth="1" min="2" max="2" width="25.0"/>
+    <col customWidth="1" min="4" max="4" width="19.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -387,19 +417,25 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3">
-        <v>28.0</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -418,47 +454,89 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.38"/>
+    <col customWidth="1" min="2" max="2" width="14.13"/>
+    <col customWidth="1" min="3" max="3" width="13.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>28.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="16.38"/>
     <col customWidth="1" min="2" max="2" width="59.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>5</v>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" ht="57.75" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
+      <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>

</xml_diff>